<commit_message>
Add invoice printing functions
</commit_message>
<xml_diff>
--- a/05-python/data/billy_test_data.xlsx
+++ b/05-python/data/billy_test_data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Customers" sheetId="1" state="visible" r:id="rId2"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
   <si>
     <t xml:space="preserve">customer_id</t>
   </si>
@@ -76,6 +76,12 @@
     <t xml:space="preserve">visa</t>
   </si>
   <si>
+    <t xml:space="preserve">2020-01-02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">amex</t>
+  </si>
+  <si>
     <t xml:space="preserve">product_id</t>
   </si>
   <si>
@@ -110,10 +116,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -166,6 +173,12 @@
       <family val="0"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -215,7 +228,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -237,6 +250,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -368,7 +389,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.609375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11"/>
@@ -765,11 +786,11 @@
   </sheetPr>
   <dimension ref="A1:D1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.75"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.01"/>
@@ -799,14 +820,27 @@
       <c r="B2" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="6" t="s">
         <v>14</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="3" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
     <row r="4" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="5" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="6" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -1829,20 +1863,20 @@
       <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.13"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1850,7 +1884,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C2" s="5" t="n">
         <v>1</v>
@@ -1861,7 +1895,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C3" s="5" t="n">
         <v>2</v>
@@ -1872,7 +1906,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C4" s="5" t="n">
         <v>3</v>
@@ -1883,7 +1917,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C5" s="5" t="n">
         <v>4</v>
@@ -1894,7 +1928,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C6" s="5" t="n">
         <v>5</v>
@@ -2089,31 +2123,31 @@
   </sheetPr>
   <dimension ref="A1:D1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="9.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="7.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="5" style="0" width="8.63"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>